<commit_message>
"Create User Account" - Update log function - Add cipher ultil class for token encrypt - Add new Login Session model - Update SQL script for login_session table - Update DB design for login_session table - Update constants
</commit_message>
<xml_diff>
--- a/doc/detail_design/db/MCS_Database_Design.xlsx
+++ b/doc/detail_design/db/MCS_Database_Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4260" yWindow="-19460" windowWidth="29020" windowHeight="16540" tabRatio="818" activeTab="6"/>
+    <workbookView xWindow="1180" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="818" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -14,115 +14,131 @@
     <sheet name="user" sheetId="5" r:id="rId5"/>
     <sheet name="article" sheetId="21" r:id="rId6"/>
     <sheet name="x_user_article" sheetId="26" r:id="rId7"/>
-    <sheet name="edition" sheetId="36" state="hidden" r:id="rId8"/>
-    <sheet name="x_edition_version" sheetId="37" state="hidden" r:id="rId9"/>
-    <sheet name="ranking(deleted)" sheetId="20" state="hidden" r:id="rId10"/>
+    <sheet name="login_session" sheetId="65" r:id="rId8"/>
+    <sheet name="edition" sheetId="36" state="hidden" r:id="rId9"/>
+    <sheet name="x_edition_version" sheetId="37" state="hidden" r:id="rId10"/>
+    <sheet name="ranking(deleted)" sheetId="20" state="hidden" r:id="rId11"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <definedNames>
     <definedName name="⑫画面" localSheetId="5">#REF!</definedName>
+    <definedName name="⑫画面" localSheetId="8">#REF!</definedName>
+    <definedName name="⑫画面" localSheetId="3">#REF!</definedName>
     <definedName name="⑫画面" localSheetId="7">#REF!</definedName>
-    <definedName name="⑫画面" localSheetId="3">#REF!</definedName>
+    <definedName name="⑫画面" localSheetId="10">#REF!</definedName>
     <definedName name="⑫画面" localSheetId="9">#REF!</definedName>
-    <definedName name="⑫画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑫画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑫画面">#REF!</definedName>
     <definedName name="②画面" localSheetId="5">#REF!</definedName>
+    <definedName name="②画面" localSheetId="8">#REF!</definedName>
+    <definedName name="②画面" localSheetId="3">#REF!</definedName>
     <definedName name="②画面" localSheetId="7">#REF!</definedName>
-    <definedName name="②画面" localSheetId="3">#REF!</definedName>
+    <definedName name="②画面" localSheetId="10">#REF!</definedName>
     <definedName name="②画面" localSheetId="9">#REF!</definedName>
-    <definedName name="②画面" localSheetId="8">#REF!</definedName>
     <definedName name="②画面" localSheetId="6">#REF!</definedName>
     <definedName name="②画面">#REF!</definedName>
     <definedName name="③画面" localSheetId="5">#REF!</definedName>
+    <definedName name="③画面" localSheetId="8">#REF!</definedName>
+    <definedName name="③画面" localSheetId="3">#REF!</definedName>
     <definedName name="③画面" localSheetId="7">#REF!</definedName>
-    <definedName name="③画面" localSheetId="3">#REF!</definedName>
+    <definedName name="③画面" localSheetId="10">#REF!</definedName>
     <definedName name="③画面" localSheetId="9">#REF!</definedName>
-    <definedName name="③画面" localSheetId="8">#REF!</definedName>
     <definedName name="③画面" localSheetId="6">#REF!</definedName>
     <definedName name="③画面">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="5">#REF!</definedName>
+    <definedName name="⑤画面" localSheetId="8">#REF!</definedName>
+    <definedName name="⑤画面" localSheetId="3">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="7">#REF!</definedName>
-    <definedName name="⑤画面" localSheetId="3">#REF!</definedName>
+    <definedName name="⑤画面" localSheetId="10">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="9">#REF!</definedName>
-    <definedName name="⑤画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑤画面">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="5">#REF!</definedName>
+    <definedName name="⑧画面" localSheetId="8">#REF!</definedName>
+    <definedName name="⑧画面" localSheetId="3">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="7">#REF!</definedName>
-    <definedName name="⑧画面" localSheetId="3">#REF!</definedName>
+    <definedName name="⑧画面" localSheetId="10">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="9">#REF!</definedName>
-    <definedName name="⑧画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑧画面">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="5">#REF!</definedName>
+    <definedName name="⑨画面" localSheetId="8">#REF!</definedName>
+    <definedName name="⑨画面" localSheetId="3">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="7">#REF!</definedName>
-    <definedName name="⑨画面" localSheetId="3">#REF!</definedName>
+    <definedName name="⑨画面" localSheetId="10">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="9">#REF!</definedName>
-    <definedName name="⑨画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑨画面">#REF!</definedName>
+    <definedName name="AAAAAA" localSheetId="8">#REF!</definedName>
+    <definedName name="AAAAAA" localSheetId="3">#REF!</definedName>
     <definedName name="AAAAAA" localSheetId="7">#REF!</definedName>
-    <definedName name="AAAAAA" localSheetId="3">#REF!</definedName>
-    <definedName name="AAAAAA" localSheetId="8">#REF!</definedName>
+    <definedName name="AAAAAA" localSheetId="9">#REF!</definedName>
     <definedName name="AAAAAA" localSheetId="6">#REF!</definedName>
     <definedName name="AAAAAA">#REF!</definedName>
+    <definedName name="as" localSheetId="8">#REF!</definedName>
+    <definedName name="as" localSheetId="3">#REF!</definedName>
     <definedName name="as" localSheetId="7">#REF!</definedName>
-    <definedName name="as" localSheetId="3">#REF!</definedName>
-    <definedName name="as" localSheetId="8">#REF!</definedName>
+    <definedName name="as" localSheetId="9">#REF!</definedName>
     <definedName name="as" localSheetId="6">#REF!</definedName>
     <definedName name="as">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="5">#REF!</definedName>
+    <definedName name="ｄｄｄｄ" localSheetId="8">#REF!</definedName>
+    <definedName name="ｄｄｄｄ" localSheetId="3">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="7">#REF!</definedName>
-    <definedName name="ｄｄｄｄ" localSheetId="3">#REF!</definedName>
+    <definedName name="ｄｄｄｄ" localSheetId="10">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="9">#REF!</definedName>
-    <definedName name="ｄｄｄｄ" localSheetId="8">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="6">#REF!</definedName>
     <definedName name="ｄｄｄｄ">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="5">#REF!</definedName>
+    <definedName name="ｄｄｄｄｄ" localSheetId="8">#REF!</definedName>
+    <definedName name="ｄｄｄｄｄ" localSheetId="3">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="7">#REF!</definedName>
-    <definedName name="ｄｄｄｄｄ" localSheetId="3">#REF!</definedName>
+    <definedName name="ｄｄｄｄｄ" localSheetId="10">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="9">#REF!</definedName>
-    <definedName name="ｄｄｄｄｄ" localSheetId="8">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="6">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ">#REF!</definedName>
     <definedName name="MySQL_DataType">[1]データタイプ!$B$2:$B$36</definedName>
     <definedName name="Oracle_DataType">[1]データタイプ!$A$2:$A$24</definedName>
     <definedName name="あ" localSheetId="5">#REF!</definedName>
+    <definedName name="あ" localSheetId="8">#REF!</definedName>
+    <definedName name="あ" localSheetId="3">#REF!</definedName>
     <definedName name="あ" localSheetId="7">#REF!</definedName>
-    <definedName name="あ" localSheetId="3">#REF!</definedName>
+    <definedName name="あ" localSheetId="10">#REF!</definedName>
     <definedName name="あ" localSheetId="9">#REF!</definedName>
-    <definedName name="あ" localSheetId="8">#REF!</definedName>
     <definedName name="あ" localSheetId="6">#REF!</definedName>
     <definedName name="あ">#REF!</definedName>
     <definedName name="ステータス" localSheetId="5">#REF!</definedName>
+    <definedName name="ステータス" localSheetId="8">#REF!</definedName>
+    <definedName name="ステータス" localSheetId="3">#REF!</definedName>
     <definedName name="ステータス" localSheetId="7">#REF!</definedName>
-    <definedName name="ステータス" localSheetId="3">#REF!</definedName>
+    <definedName name="ステータス" localSheetId="10">#REF!</definedName>
     <definedName name="ステータス" localSheetId="9">#REF!</definedName>
-    <definedName name="ステータス" localSheetId="8">#REF!</definedName>
     <definedName name="ステータス" localSheetId="6">#REF!</definedName>
     <definedName name="ステータス">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="5">#REF!</definedName>
+    <definedName name="画面一覧" localSheetId="8">#REF!</definedName>
+    <definedName name="画面一覧" localSheetId="3">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="7">#REF!</definedName>
-    <definedName name="画面一覧" localSheetId="3">#REF!</definedName>
+    <definedName name="画面一覧" localSheetId="10">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="9">#REF!</definedName>
-    <definedName name="画面一覧" localSheetId="8">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="6">#REF!</definedName>
     <definedName name="画面一覧">#REF!</definedName>
     <definedName name="項番17" localSheetId="5">#REF!</definedName>
+    <definedName name="項番17" localSheetId="8">#REF!</definedName>
+    <definedName name="項番17" localSheetId="3">#REF!</definedName>
     <definedName name="項番17" localSheetId="7">#REF!</definedName>
-    <definedName name="項番17" localSheetId="3">#REF!</definedName>
+    <definedName name="項番17" localSheetId="10">#REF!</definedName>
     <definedName name="項番17" localSheetId="9">#REF!</definedName>
-    <definedName name="項番17" localSheetId="8">#REF!</definedName>
     <definedName name="項番17" localSheetId="6">#REF!</definedName>
     <definedName name="項番17">#REF!</definedName>
     <definedName name="項番3" localSheetId="5">#REF!</definedName>
+    <definedName name="項番3" localSheetId="8">#REF!</definedName>
+    <definedName name="項番3" localSheetId="3">#REF!</definedName>
     <definedName name="項番3" localSheetId="7">#REF!</definedName>
-    <definedName name="項番3" localSheetId="3">#REF!</definedName>
+    <definedName name="項番3" localSheetId="10">#REF!</definedName>
     <definedName name="項番3" localSheetId="9">#REF!</definedName>
-    <definedName name="項番3" localSheetId="8">#REF!</definedName>
     <definedName name="項番3" localSheetId="6">#REF!</definedName>
     <definedName name="項番3">#REF!</definedName>
   </definedNames>
@@ -136,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="190">
   <si>
     <t>No</t>
   </si>
@@ -695,6 +711,21 @@
   </si>
   <si>
     <t>Moi</t>
+  </si>
+  <si>
+    <t>Login session data</t>
+  </si>
+  <si>
+    <t>03/11/2014</t>
+  </si>
+  <si>
+    <t>login_session</t>
+  </si>
+  <si>
+    <t>Ref system ID.</t>
+  </si>
+  <si>
+    <t>encrypt format =  "secrectkey@access_id@player_id@Date(UNIX TIME)"</t>
   </si>
 </sst>
 </file>
@@ -1930,7 +1961,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="441">
+  <cellStyleXfs count="443">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3251,8 +3282,14 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="256">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3766,6 +3803,39 @@
     <xf numFmtId="49" fontId="24" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3776,12 +3846,75 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3797,67 +3930,22 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3890,30 +3978,6 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3926,6 +3990,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3944,41 +4014,26 @@
     <xf numFmtId="49" fontId="24" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="441">
+  <cellStyles count="443">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -4412,6 +4467,8 @@
     <cellStyle name="Followed Hyperlink" xfId="438" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="439" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ハイパーリンク 2" xfId="4"/>
@@ -5714,29 +5771,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="185"/>
-      <c r="P13" s="185"/>
-      <c r="Q13" s="185"/>
-      <c r="R13" s="185"/>
-      <c r="S13" s="185"/>
-      <c r="T13" s="185"/>
-      <c r="U13" s="185"/>
-      <c r="V13" s="185"/>
-      <c r="W13" s="185"/>
-      <c r="X13" s="185"/>
-      <c r="Y13" s="185"/>
-      <c r="Z13" s="185"/>
-      <c r="AA13" s="185"/>
-      <c r="AB13" s="185"/>
-      <c r="AC13" s="185"/>
-      <c r="AD13" s="185"/>
-      <c r="AE13" s="185"/>
-      <c r="AF13" s="185"/>
-      <c r="AG13" s="185"/>
-      <c r="AH13" s="185"/>
-      <c r="AI13" s="185"/>
-      <c r="AJ13" s="185"/>
-      <c r="AK13" s="185"/>
+      <c r="O13" s="196"/>
+      <c r="P13" s="196"/>
+      <c r="Q13" s="196"/>
+      <c r="R13" s="196"/>
+      <c r="S13" s="196"/>
+      <c r="T13" s="196"/>
+      <c r="U13" s="196"/>
+      <c r="V13" s="196"/>
+      <c r="W13" s="196"/>
+      <c r="X13" s="196"/>
+      <c r="Y13" s="196"/>
+      <c r="Z13" s="196"/>
+      <c r="AA13" s="196"/>
+      <c r="AB13" s="196"/>
+      <c r="AC13" s="196"/>
+      <c r="AD13" s="196"/>
+      <c r="AE13" s="196"/>
+      <c r="AF13" s="196"/>
+      <c r="AG13" s="196"/>
+      <c r="AH13" s="196"/>
+      <c r="AI13" s="196"/>
+      <c r="AJ13" s="196"/>
+      <c r="AK13" s="196"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5768,29 +5825,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="185"/>
-      <c r="P14" s="185"/>
-      <c r="Q14" s="185"/>
-      <c r="R14" s="185"/>
-      <c r="S14" s="185"/>
-      <c r="T14" s="185"/>
-      <c r="U14" s="185"/>
-      <c r="V14" s="185"/>
-      <c r="W14" s="185"/>
-      <c r="X14" s="185"/>
-      <c r="Y14" s="185"/>
-      <c r="Z14" s="185"/>
-      <c r="AA14" s="185"/>
-      <c r="AB14" s="185"/>
-      <c r="AC14" s="185"/>
-      <c r="AD14" s="185"/>
-      <c r="AE14" s="185"/>
-      <c r="AF14" s="185"/>
-      <c r="AG14" s="185"/>
-      <c r="AH14" s="185"/>
-      <c r="AI14" s="185"/>
-      <c r="AJ14" s="185"/>
-      <c r="AK14" s="185"/>
+      <c r="O14" s="196"/>
+      <c r="P14" s="196"/>
+      <c r="Q14" s="196"/>
+      <c r="R14" s="196"/>
+      <c r="S14" s="196"/>
+      <c r="T14" s="196"/>
+      <c r="U14" s="196"/>
+      <c r="V14" s="196"/>
+      <c r="W14" s="196"/>
+      <c r="X14" s="196"/>
+      <c r="Y14" s="196"/>
+      <c r="Z14" s="196"/>
+      <c r="AA14" s="196"/>
+      <c r="AB14" s="196"/>
+      <c r="AC14" s="196"/>
+      <c r="AD14" s="196"/>
+      <c r="AE14" s="196"/>
+      <c r="AF14" s="196"/>
+      <c r="AG14" s="196"/>
+      <c r="AH14" s="196"/>
+      <c r="AI14" s="196"/>
+      <c r="AJ14" s="196"/>
+      <c r="AK14" s="196"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5818,43 +5875,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="186" t="s">
+      <c r="K15" s="197" t="s">
         <v>108</v>
       </c>
-      <c r="L15" s="186"/>
-      <c r="M15" s="186"/>
-      <c r="N15" s="186"/>
-      <c r="O15" s="186"/>
-      <c r="P15" s="186"/>
-      <c r="Q15" s="186"/>
-      <c r="R15" s="186"/>
-      <c r="S15" s="186"/>
-      <c r="T15" s="186"/>
-      <c r="U15" s="186"/>
-      <c r="V15" s="186"/>
-      <c r="W15" s="186"/>
-      <c r="X15" s="186"/>
-      <c r="Y15" s="186"/>
-      <c r="Z15" s="186"/>
-      <c r="AA15" s="186"/>
-      <c r="AB15" s="186"/>
-      <c r="AC15" s="186"/>
-      <c r="AD15" s="186"/>
-      <c r="AE15" s="186"/>
-      <c r="AF15" s="186"/>
-      <c r="AG15" s="186"/>
-      <c r="AH15" s="186"/>
-      <c r="AI15" s="186"/>
-      <c r="AJ15" s="186"/>
-      <c r="AK15" s="186"/>
-      <c r="AL15" s="186"/>
-      <c r="AM15" s="186"/>
-      <c r="AN15" s="186"/>
-      <c r="AO15" s="186"/>
-      <c r="AP15" s="186"/>
-      <c r="AQ15" s="186"/>
-      <c r="AR15" s="186"/>
-      <c r="AS15" s="186"/>
+      <c r="L15" s="197"/>
+      <c r="M15" s="197"/>
+      <c r="N15" s="197"/>
+      <c r="O15" s="197"/>
+      <c r="P15" s="197"/>
+      <c r="Q15" s="197"/>
+      <c r="R15" s="197"/>
+      <c r="S15" s="197"/>
+      <c r="T15" s="197"/>
+      <c r="U15" s="197"/>
+      <c r="V15" s="197"/>
+      <c r="W15" s="197"/>
+      <c r="X15" s="197"/>
+      <c r="Y15" s="197"/>
+      <c r="Z15" s="197"/>
+      <c r="AA15" s="197"/>
+      <c r="AB15" s="197"/>
+      <c r="AC15" s="197"/>
+      <c r="AD15" s="197"/>
+      <c r="AE15" s="197"/>
+      <c r="AF15" s="197"/>
+      <c r="AG15" s="197"/>
+      <c r="AH15" s="197"/>
+      <c r="AI15" s="197"/>
+      <c r="AJ15" s="197"/>
+      <c r="AK15" s="197"/>
+      <c r="AL15" s="197"/>
+      <c r="AM15" s="197"/>
+      <c r="AN15" s="197"/>
+      <c r="AO15" s="197"/>
+      <c r="AP15" s="197"/>
+      <c r="AQ15" s="197"/>
+      <c r="AR15" s="197"/>
+      <c r="AS15" s="197"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5874,41 +5931,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="186"/>
-      <c r="L16" s="186"/>
-      <c r="M16" s="186"/>
-      <c r="N16" s="186"/>
-      <c r="O16" s="186"/>
-      <c r="P16" s="186"/>
-      <c r="Q16" s="186"/>
-      <c r="R16" s="186"/>
-      <c r="S16" s="186"/>
-      <c r="T16" s="186"/>
-      <c r="U16" s="186"/>
-      <c r="V16" s="186"/>
-      <c r="W16" s="186"/>
-      <c r="X16" s="186"/>
-      <c r="Y16" s="186"/>
-      <c r="Z16" s="186"/>
-      <c r="AA16" s="186"/>
-      <c r="AB16" s="186"/>
-      <c r="AC16" s="186"/>
-      <c r="AD16" s="186"/>
-      <c r="AE16" s="186"/>
-      <c r="AF16" s="186"/>
-      <c r="AG16" s="186"/>
-      <c r="AH16" s="186"/>
-      <c r="AI16" s="186"/>
-      <c r="AJ16" s="186"/>
-      <c r="AK16" s="186"/>
-      <c r="AL16" s="186"/>
-      <c r="AM16" s="186"/>
-      <c r="AN16" s="186"/>
-      <c r="AO16" s="186"/>
-      <c r="AP16" s="186"/>
-      <c r="AQ16" s="186"/>
-      <c r="AR16" s="186"/>
-      <c r="AS16" s="186"/>
+      <c r="K16" s="197"/>
+      <c r="L16" s="197"/>
+      <c r="M16" s="197"/>
+      <c r="N16" s="197"/>
+      <c r="O16" s="197"/>
+      <c r="P16" s="197"/>
+      <c r="Q16" s="197"/>
+      <c r="R16" s="197"/>
+      <c r="S16" s="197"/>
+      <c r="T16" s="197"/>
+      <c r="U16" s="197"/>
+      <c r="V16" s="197"/>
+      <c r="W16" s="197"/>
+      <c r="X16" s="197"/>
+      <c r="Y16" s="197"/>
+      <c r="Z16" s="197"/>
+      <c r="AA16" s="197"/>
+      <c r="AB16" s="197"/>
+      <c r="AC16" s="197"/>
+      <c r="AD16" s="197"/>
+      <c r="AE16" s="197"/>
+      <c r="AF16" s="197"/>
+      <c r="AG16" s="197"/>
+      <c r="AH16" s="197"/>
+      <c r="AI16" s="197"/>
+      <c r="AJ16" s="197"/>
+      <c r="AK16" s="197"/>
+      <c r="AL16" s="197"/>
+      <c r="AM16" s="197"/>
+      <c r="AN16" s="197"/>
+      <c r="AO16" s="197"/>
+      <c r="AP16" s="197"/>
+      <c r="AQ16" s="197"/>
+      <c r="AR16" s="197"/>
+      <c r="AS16" s="197"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6497,14 +6554,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="187">
+      <c r="AN27" s="198">
         <v>41922</v>
       </c>
-      <c r="AO27" s="187"/>
-      <c r="AP27" s="187"/>
-      <c r="AQ27" s="187"/>
-      <c r="AR27" s="187"/>
-      <c r="AS27" s="187"/>
+      <c r="AO27" s="198"/>
+      <c r="AP27" s="198"/>
+      <c r="AQ27" s="198"/>
+      <c r="AR27" s="198"/>
+      <c r="AS27" s="198"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -6966,6 +7023,386 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FF008000"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="18" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" style="18" customWidth="1"/>
+    <col min="5" max="6" width="10.1640625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="12" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13">
+      <c r="B2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="200" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="201"/>
+      <c r="E2" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="200" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="204"/>
+    </row>
+    <row r="3" spans="1:7" ht="13">
+      <c r="B3" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="202" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="206"/>
+    </row>
+    <row r="4" spans="1:7" ht="13">
+      <c r="B4" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="202" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="203"/>
+      <c r="E4" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="202"/>
+      <c r="G4" s="206"/>
+    </row>
+    <row r="5" spans="1:7" ht="13">
+      <c r="B5" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="202" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="203"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="206"/>
+    </row>
+    <row r="6" spans="1:7" ht="13">
+      <c r="B6" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="202" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="203"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="206"/>
+    </row>
+    <row r="7" spans="1:7" ht="13">
+      <c r="B7" s="211" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212"/>
+      <c r="G7" s="213"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="B8" s="214" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="216"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="B9" s="217"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
+    </row>
+    <row r="10" spans="1:7" ht="12" thickBot="1">
+      <c r="B10" s="218"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="220"/>
+    </row>
+    <row r="12" spans="1:7" ht="12" thickBot="1">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="14">
+        <v>1</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="15">
+        <f>A14+1</f>
+        <v>2</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="23"/>
+      <c r="G15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" ht="12" thickBot="1">
+      <c r="A16" s="16">
+        <f t="shared" ref="A16" si="0">A15+1</f>
+        <v>3</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="62" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="12" thickBot="1">
+      <c r="A18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="207" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="208"/>
+      <c r="E19" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="13">
+      <c r="A20" s="14">
+        <v>1</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="221" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="222"/>
+      <c r="E20" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="1:7" ht="14" thickBot="1">
+      <c r="A21" s="16">
+        <v>2</v>
+      </c>
+      <c r="B21" s="26"/>
+      <c r="C21" s="250" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="251"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="28"/>
+    </row>
+    <row r="23" spans="1:7" ht="12" thickBot="1">
+      <c r="A23" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="14" thickBot="1">
+      <c r="A24" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="209" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="210"/>
+      <c r="E24" s="209" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="223"/>
+      <c r="G24" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="12" thickBot="1">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14" thickBot="1">
+      <c r="A27" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="209" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="210"/>
+      <c r="E27" s="209" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="223"/>
+      <c r="G27" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14" thickBot="1">
+      <c r="A28" s="16">
+        <v>1</v>
+      </c>
+      <c r="B28" s="26"/>
+      <c r="C28" s="250"/>
+      <c r="D28" s="251"/>
+      <c r="E28" s="252"/>
+      <c r="F28" s="253"/>
+      <c r="G28" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+  </mergeCells>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <headerFooter>
+    <oddHeader>&amp;Lテーブル定義書&amp;R&amp;D</oddHeader>
+    <oddFooter>&amp;C&amp;P/&amp;N</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -6994,103 +7431,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="210" t="s">
+      <c r="C2" s="200" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="215"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="243" t="s">
+      <c r="F2" s="254" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="244"/>
+      <c r="G2" s="255"/>
     </row>
     <row r="3" spans="1:14" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="205" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="213"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="214" t="s">
+      <c r="C4" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="216"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="214"/>
-      <c r="G4" s="213"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="206"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="214" t="s">
+      <c r="C5" s="202" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="216"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="214"/>
-      <c r="G5" s="213"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="206"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="214" t="s">
+      <c r="C6" s="202" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="216"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="214"/>
-      <c r="G6" s="213"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="206"/>
     </row>
     <row r="7" spans="1:14" ht="13">
-      <c r="B7" s="198" t="s">
+      <c r="B7" s="211" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="200"/>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212"/>
+      <c r="G7" s="213"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="201"/>
-      <c r="C8" s="202"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="203"/>
+      <c r="B8" s="214"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="216"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="204"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="203"/>
+      <c r="B9" s="217"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="205"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="207"/>
+      <c r="B10" s="218"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="220"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="113"/>
@@ -7306,10 +7743,10 @@
       <c r="B21" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C21" s="196" t="s">
+      <c r="C21" s="207" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="197"/>
+      <c r="D21" s="208"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -7333,10 +7770,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="208" t="s">
+      <c r="C22" s="221" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="209"/>
+      <c r="D22" s="222"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -7356,10 +7793,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="194" t="s">
+      <c r="C23" s="226" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="195"/>
+      <c r="D23" s="227"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -7377,10 +7814,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="239" t="s">
+      <c r="C24" s="250" t="s">
         <v>70</v>
       </c>
-      <c r="D24" s="240"/>
+      <c r="D24" s="251"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -7419,14 +7856,14 @@
       <c r="B27" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="189" t="s">
+      <c r="C27" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="190"/>
-      <c r="E27" s="189" t="s">
+      <c r="D27" s="210"/>
+      <c r="E27" s="209" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="191"/>
+      <c r="F27" s="223"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -7463,14 +7900,14 @@
       <c r="B30" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="189" t="s">
+      <c r="C30" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D30" s="190"/>
-      <c r="E30" s="189" t="s">
+      <c r="D30" s="210"/>
+      <c r="E30" s="209" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="191"/>
+      <c r="F30" s="223"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -7486,14 +7923,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="208" t="s">
+      <c r="C31" s="221" t="s">
         <v>78</v>
       </c>
-      <c r="D31" s="209"/>
-      <c r="E31" s="194" t="s">
+      <c r="D31" s="222"/>
+      <c r="E31" s="226" t="s">
         <v>76</v>
       </c>
-      <c r="F31" s="195"/>
+      <c r="F31" s="227"/>
       <c r="G31" s="53" t="s">
         <v>78</v>
       </c>
@@ -7509,14 +7946,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="221" t="s">
+      <c r="C32" s="238" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="222"/>
-      <c r="E32" s="241" t="s">
+      <c r="D32" s="239"/>
+      <c r="E32" s="252" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="242"/>
+      <c r="F32" s="253"/>
       <c r="G32" s="55" t="s">
         <v>53</v>
       </c>
@@ -7569,14 +8006,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -7593,6 +8022,14 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7911,11 +8348,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12" thickBot="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="199" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
     </row>
     <row r="2" spans="1:3" ht="12" thickBot="1">
       <c r="A2" s="166" t="s">
@@ -7935,7 +8372,7 @@
       <c r="B3" s="170" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="245" t="s">
+      <c r="C3" s="185" t="s">
         <v>110</v>
       </c>
     </row>
@@ -8190,11 +8627,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12" thickBot="1">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="199" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="188"/>
-      <c r="C1" s="188"/>
+      <c r="B1" s="199"/>
+      <c r="C1" s="199"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8222,7 +8659,7 @@
   </sheetPr>
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
@@ -8253,103 +8690,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="210" t="s">
+      <c r="C2" s="200" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="215"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="210" t="s">
+      <c r="F2" s="200" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="211"/>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="205" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="213"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="214" t="s">
+      <c r="C4" s="202" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="216"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="214"/>
-      <c r="G4" s="213"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="206"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="214" t="s">
+      <c r="C5" s="202" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="216"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="214"/>
-      <c r="G5" s="213"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="206"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="214" t="s">
+      <c r="C6" s="202" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="216"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="214"/>
-      <c r="G6" s="213"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="206"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="198" t="s">
+      <c r="B7" s="211" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="200"/>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212"/>
+      <c r="G7" s="213"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="201"/>
-      <c r="C8" s="202"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="203"/>
+      <c r="B8" s="214"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="216"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="204"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="203"/>
+      <c r="B9" s="217"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="205"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="207"/>
+      <c r="B10" s="218"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="220"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8451,7 +8888,7 @@
       <c r="M14" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="N14" s="255" t="s">
+      <c r="N14" s="195" t="s">
         <v>179</v>
       </c>
       <c r="O14" s="13" t="s">
@@ -8507,7 +8944,7 @@
       <c r="M15" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="N15" s="255" t="s">
+      <c r="N15" s="195" t="s">
         <v>182</v>
       </c>
       <c r="O15" s="13" t="s">
@@ -8696,22 +9133,22 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B24" s="246" t="s">
+      <c r="B24" s="186" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="247" t="s">
+      <c r="C24" s="187" t="s">
         <v>6</v>
       </c>
-      <c r="D24" s="247" t="s">
+      <c r="D24" s="187" t="s">
         <v>174</v>
       </c>
-      <c r="E24" s="248" t="s">
+      <c r="E24" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="250" t="s">
+      <c r="F24" s="190" t="s">
         <v>100</v>
       </c>
-      <c r="G24" s="249" t="s">
+      <c r="G24" s="189" t="s">
         <v>172</v>
       </c>
     </row>
@@ -8727,10 +9164,10 @@
       <c r="B27" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="196" t="s">
+      <c r="C27" s="207" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="197"/>
+      <c r="D27" s="208"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -8748,10 +9185,10 @@
       <c r="B28" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="208" t="s">
+      <c r="C28" s="221" t="s">
         <v>152</v>
       </c>
-      <c r="D28" s="209"/>
+      <c r="D28" s="222"/>
       <c r="E28" s="46" t="s">
         <v>3</v>
       </c>
@@ -8765,10 +9202,10 @@
         <v>2</v>
       </c>
       <c r="B29" s="51"/>
-      <c r="C29" s="194" t="s">
+      <c r="C29" s="226" t="s">
         <v>118</v>
       </c>
-      <c r="D29" s="195"/>
+      <c r="D29" s="227"/>
       <c r="E29" s="52"/>
       <c r="F29" s="52" t="s">
         <v>3</v>
@@ -8780,8 +9217,8 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="192"/>
-      <c r="D30" s="193"/>
+      <c r="C30" s="224"/>
+      <c r="D30" s="225"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="55"/>
@@ -8798,14 +9235,14 @@
       <c r="B33" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="189" t="s">
+      <c r="C33" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="190"/>
-      <c r="E33" s="189" t="s">
+      <c r="D33" s="210"/>
+      <c r="E33" s="209" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="191"/>
+      <c r="F33" s="223"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -8822,40 +9259,40 @@
       <c r="B36" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="189" t="s">
+      <c r="C36" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D36" s="190"/>
-      <c r="E36" s="189" t="s">
+      <c r="D36" s="210"/>
+      <c r="E36" s="209" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="191"/>
+      <c r="F36" s="223"/>
       <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -8883,8 +9320,8 @@
   </sheetPr>
   <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -8919,108 +9356,108 @@
       <c r="B2" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="210" t="s">
+      <c r="C2" s="200" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="215"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="210" t="s">
+      <c r="F2" s="200" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="211"/>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:14" ht="13">
       <c r="A3" s="94"/>
       <c r="B3" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="205" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="213"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="A4" s="94"/>
       <c r="B4" s="96" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="214" t="s">
+      <c r="C4" s="202" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="216"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="214"/>
-      <c r="G4" s="213"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="206"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="A5" s="94"/>
       <c r="B5" s="96" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="227" t="s">
+      <c r="C5" s="228" t="s">
         <v>120</v>
       </c>
-      <c r="D5" s="228"/>
+      <c r="D5" s="229"/>
       <c r="E5" s="97"/>
-      <c r="F5" s="227"/>
-      <c r="G5" s="229"/>
+      <c r="F5" s="228"/>
+      <c r="G5" s="230"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="A6" s="94"/>
       <c r="B6" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="228" t="s">
         <v>121</v>
       </c>
-      <c r="D6" s="228"/>
+      <c r="D6" s="229"/>
       <c r="E6" s="98"/>
-      <c r="F6" s="227"/>
-      <c r="G6" s="229"/>
+      <c r="F6" s="228"/>
+      <c r="G6" s="230"/>
     </row>
     <row r="7" spans="1:14" ht="13">
       <c r="A7" s="94"/>
-      <c r="B7" s="230" t="s">
+      <c r="B7" s="231" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="231"/>
-      <c r="D7" s="231"/>
-      <c r="E7" s="231"/>
-      <c r="F7" s="231"/>
-      <c r="G7" s="232"/>
+      <c r="C7" s="232"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="232"/>
+      <c r="F7" s="232"/>
+      <c r="G7" s="233"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="201"/>
-      <c r="C8" s="202"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="203"/>
+      <c r="B8" s="214"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="216"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="204"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="203"/>
+      <c r="B9" s="217"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="205"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="207"/>
+      <c r="B10" s="218"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="220"/>
     </row>
     <row r="12" spans="1:14" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9213,22 +9650,22 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B19" s="246" t="s">
+      <c r="B19" s="186" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="247" t="s">
+      <c r="C19" s="187" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="247" t="s">
+      <c r="D19" s="187" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="248" t="s">
+      <c r="E19" s="188" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="250" t="s">
+      <c r="F19" s="190" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="249" t="s">
+      <c r="G19" s="189" t="s">
         <v>171</v>
       </c>
     </row>
@@ -9244,10 +9681,10 @@
       <c r="B22" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="196" t="s">
+      <c r="C22" s="207" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="197"/>
+      <c r="D22" s="208"/>
       <c r="E22" s="34" t="s">
         <v>33</v>
       </c>
@@ -9265,10 +9702,10 @@
       <c r="B23" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="221" t="s">
+      <c r="C23" s="238" t="s">
         <v>152</v>
       </c>
-      <c r="D23" s="222"/>
+      <c r="D23" s="239"/>
       <c r="E23" s="58" t="s">
         <v>3</v>
       </c>
@@ -9289,14 +9726,14 @@
       <c r="B26" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="189" t="s">
+      <c r="C26" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D26" s="190"/>
-      <c r="E26" s="189" t="s">
+      <c r="D26" s="210"/>
+      <c r="E26" s="209" t="s">
         <v>36</v>
       </c>
-      <c r="F26" s="191"/>
+      <c r="F26" s="223"/>
       <c r="G26" s="38" t="s">
         <v>38</v>
       </c>
@@ -9306,10 +9743,10 @@
         <v>1</v>
       </c>
       <c r="B27" s="144"/>
-      <c r="C27" s="223"/>
-      <c r="D27" s="224"/>
-      <c r="E27" s="225"/>
-      <c r="F27" s="226"/>
+      <c r="C27" s="240"/>
+      <c r="D27" s="241"/>
+      <c r="E27" s="242"/>
+      <c r="F27" s="243"/>
       <c r="G27" s="145"/>
     </row>
     <row r="28" spans="1:7" ht="14" thickBot="1">
@@ -9317,10 +9754,10 @@
         <v>2</v>
       </c>
       <c r="B28" s="147"/>
-      <c r="C28" s="217"/>
-      <c r="D28" s="218"/>
-      <c r="E28" s="219"/>
-      <c r="F28" s="220"/>
+      <c r="C28" s="234"/>
+      <c r="D28" s="235"/>
+      <c r="E28" s="236"/>
+      <c r="F28" s="237"/>
       <c r="G28" s="148"/>
     </row>
     <row r="30" spans="1:7" ht="12" thickBot="1">
@@ -9335,31 +9772,20 @@
       <c r="B31" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="189" t="s">
+      <c r="C31" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="190"/>
-      <c r="E31" s="189" t="s">
+      <c r="D31" s="210"/>
+      <c r="E31" s="209" t="s">
         <v>37</v>
       </c>
-      <c r="F31" s="191"/>
+      <c r="F31" s="223"/>
       <c r="G31" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="C28:D28"/>
@@ -9371,6 +9797,17 @@
     <mergeCell ref="E26:F26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="E27:F27"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9394,8 +9831,8 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView topLeftCell="A5" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -9404,7 +9841,7 @@
     <col min="2" max="2" width="16.6640625" style="18" customWidth="1"/>
     <col min="3" max="4" width="14.6640625" style="18" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="251" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="191" customWidth="1"/>
     <col min="7" max="7" width="28.6640625" style="18" customWidth="1"/>
     <col min="8" max="10" width="8.83203125" style="13"/>
     <col min="11" max="11" width="11" style="13" customWidth="1"/>
@@ -9424,103 +9861,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="210" t="s">
+      <c r="C2" s="200" t="s">
         <v>111</v>
       </c>
-      <c r="D2" s="215"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="210" t="s">
+      <c r="F2" s="200" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="211"/>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:15" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="212" t="s">
+      <c r="F3" s="205" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="213"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:15" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="214" t="s">
+      <c r="C4" s="202" t="s">
         <v>113</v>
       </c>
-      <c r="D4" s="216"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="214"/>
-      <c r="G4" s="213"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="206"/>
     </row>
     <row r="5" spans="1:15" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="214" t="s">
+      <c r="C5" s="202" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="216"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="214"/>
-      <c r="G5" s="213"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="206"/>
     </row>
     <row r="6" spans="1:15" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="214" t="s">
+      <c r="C6" s="202" t="s">
         <v>130</v>
       </c>
-      <c r="D6" s="216"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="214"/>
-      <c r="G6" s="213"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="206"/>
     </row>
     <row r="7" spans="1:15" ht="13">
-      <c r="B7" s="198" t="s">
+      <c r="B7" s="211" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="200"/>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212"/>
+      <c r="G7" s="213"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="B8" s="201"/>
-      <c r="C8" s="202"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="203"/>
+      <c r="B8" s="214"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="216"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="B9" s="204"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="203"/>
+      <c r="B9" s="217"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
     </row>
     <row r="10" spans="1:15" ht="12" thickBot="1">
-      <c r="B10" s="205"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="207"/>
+      <c r="B10" s="218"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="220"/>
     </row>
     <row r="12" spans="1:15" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9590,7 +10027,7 @@
       <c r="E14" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="252"/>
+      <c r="F14" s="192"/>
       <c r="G14" s="77" t="s">
         <v>51</v>
       </c>
@@ -9633,7 +10070,7 @@
       <c r="E15" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F15" s="253"/>
+      <c r="F15" s="193"/>
       <c r="G15" s="84"/>
       <c r="I15" s="13">
         <v>2</v>
@@ -9674,7 +10111,7 @@
       <c r="E16" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="253"/>
+      <c r="F16" s="193"/>
       <c r="G16" s="84"/>
       <c r="I16" s="13">
         <v>3</v>
@@ -9715,7 +10152,7 @@
       <c r="E17" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="253" t="s">
+      <c r="F17" s="193" t="s">
         <v>4</v>
       </c>
       <c r="G17" s="84" t="s">
@@ -9760,7 +10197,7 @@
       <c r="E18" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="253"/>
+      <c r="F18" s="193"/>
       <c r="G18" s="84"/>
       <c r="I18" s="13">
         <v>5</v>
@@ -9801,7 +10238,7 @@
       <c r="E19" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="253"/>
+      <c r="F19" s="193"/>
       <c r="G19" s="84"/>
       <c r="I19" s="13">
         <v>6</v>
@@ -9842,7 +10279,7 @@
       <c r="E20" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="253"/>
+      <c r="F20" s="193"/>
       <c r="G20" s="84"/>
       <c r="I20" s="13">
         <v>7</v>
@@ -9857,7 +10294,7 @@
       <c r="C21" s="86"/>
       <c r="D21" s="68"/>
       <c r="E21" s="87"/>
-      <c r="F21" s="254"/>
+      <c r="F21" s="194"/>
       <c r="G21" s="150"/>
     </row>
     <row r="23" spans="1:15" ht="12" thickBot="1">
@@ -9872,10 +10309,10 @@
       <c r="B24" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="196" t="s">
+      <c r="C24" s="207" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="197"/>
+      <c r="D24" s="208"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -9893,10 +10330,10 @@
       <c r="B25" s="89" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="237" t="s">
+      <c r="C25" s="246" t="s">
         <v>152</v>
       </c>
-      <c r="D25" s="238"/>
+      <c r="D25" s="247"/>
       <c r="E25" s="90" t="s">
         <v>3</v>
       </c>
@@ -9931,8 +10368,8 @@
         <v>2</v>
       </c>
       <c r="B26" s="68"/>
-      <c r="C26" s="233"/>
-      <c r="D26" s="234"/>
+      <c r="C26" s="248"/>
+      <c r="D26" s="249"/>
       <c r="E26" s="69"/>
       <c r="F26" s="69"/>
       <c r="G26" s="70"/>
@@ -10014,14 +10451,14 @@
       <c r="B29" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="189" t="s">
+      <c r="C29" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="190"/>
-      <c r="E29" s="189" t="s">
+      <c r="D29" s="210"/>
+      <c r="E29" s="209" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="191"/>
+      <c r="F29" s="223"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -10052,14 +10489,14 @@
         <v>1</v>
       </c>
       <c r="B30" s="19"/>
-      <c r="C30" s="208" t="s">
+      <c r="C30" s="221" t="s">
         <v>116</v>
       </c>
-      <c r="D30" s="209"/>
-      <c r="E30" s="235" t="s">
+      <c r="D30" s="222"/>
+      <c r="E30" s="244" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="236"/>
+      <c r="F30" s="245"/>
       <c r="G30" s="20" t="s">
         <v>152</v>
       </c>
@@ -10090,14 +10527,14 @@
         <v>2</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="194" t="s">
+      <c r="C31" s="226" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="195"/>
-      <c r="E31" s="194" t="s">
+      <c r="D31" s="227"/>
+      <c r="E31" s="226" t="s">
         <v>121</v>
       </c>
-      <c r="F31" s="195"/>
+      <c r="F31" s="227"/>
       <c r="G31" s="53" t="s">
         <v>152</v>
       </c>
@@ -10128,10 +10565,10 @@
         <v>3</v>
       </c>
       <c r="B32" s="161"/>
-      <c r="C32" s="192"/>
-      <c r="D32" s="193"/>
-      <c r="E32" s="192"/>
-      <c r="F32" s="193"/>
+      <c r="C32" s="224"/>
+      <c r="D32" s="225"/>
+      <c r="E32" s="224"/>
+      <c r="F32" s="225"/>
       <c r="G32" s="162"/>
       <c r="I32" s="13">
         <v>8</v>
@@ -10167,20 +10604,29 @@
       <c r="B35" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="189" t="s">
+      <c r="C35" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D35" s="190"/>
-      <c r="E35" s="189" t="s">
+      <c r="D35" s="210"/>
+      <c r="E35" s="209" t="s">
         <v>37</v>
       </c>
-      <c r="F35" s="191"/>
+      <c r="F35" s="223"/>
       <c r="G35" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="E31:F31"/>
     <mergeCell ref="C35:D35"/>
@@ -10197,15 +10643,6 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10223,6 +10660,525 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor rgb="FFFFFF00"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="18" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" style="18" customWidth="1"/>
+    <col min="5" max="6" width="10.1640625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.83203125" style="13"/>
+    <col min="11" max="11" width="19.33203125" style="13" customWidth="1"/>
+    <col min="12" max="13" width="17" style="13" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="13" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="12" thickBot="1">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="13">
+      <c r="B2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="200" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="201"/>
+      <c r="E2" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="200" t="s">
+        <v>107</v>
+      </c>
+      <c r="G2" s="204"/>
+    </row>
+    <row r="3" spans="1:14" ht="13">
+      <c r="B3" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
+      <c r="E3" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="205" t="s">
+        <v>186</v>
+      </c>
+      <c r="G3" s="206"/>
+    </row>
+    <row r="4" spans="1:14" ht="13">
+      <c r="B4" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="202" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="203"/>
+      <c r="E4" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="202"/>
+      <c r="G4" s="206"/>
+    </row>
+    <row r="5" spans="1:14" ht="13">
+      <c r="B5" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="202" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="203"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="206"/>
+    </row>
+    <row r="6" spans="1:14" ht="13">
+      <c r="B6" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="202" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="203"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="206"/>
+    </row>
+    <row r="7" spans="1:14" ht="13">
+      <c r="B7" s="211" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212"/>
+      <c r="G7" s="213"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="B8" s="214"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="216"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="B9" s="217"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
+    </row>
+    <row r="10" spans="1:14" ht="12" thickBot="1">
+      <c r="B10" s="218"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="220"/>
+    </row>
+    <row r="12" spans="1:14" ht="12" thickBot="1">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="178" t="s">
+        <v>152</v>
+      </c>
+      <c r="J13" s="178" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="178" t="s">
+        <v>168</v>
+      </c>
+      <c r="L13" s="178" t="s">
+        <v>165</v>
+      </c>
+      <c r="M13" s="178" t="s">
+        <v>101</v>
+      </c>
+      <c r="N13" s="178" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="71">
+        <v>1</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>153</v>
+      </c>
+      <c r="C14" s="64" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="67"/>
+      <c r="G14" s="149" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="113"/>
+      <c r="I14" s="13">
+        <v>1</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="L14" s="175">
+        <v>41922.465277777781</v>
+      </c>
+      <c r="M14" s="175">
+        <v>41922.465277777781</v>
+      </c>
+      <c r="N14" s="175">
+        <v>41922.465277777781</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="59">
+        <f>A14+1</f>
+        <v>2</v>
+      </c>
+      <c r="B15" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="259" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="67"/>
+      <c r="G15" s="152" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" s="113"/>
+      <c r="I15" s="13">
+        <v>2</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="L15" s="175">
+        <v>41922.46875</v>
+      </c>
+      <c r="M15" s="175">
+        <v>41922.46875</v>
+      </c>
+      <c r="N15" s="175">
+        <v>41922.46875</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="33">
+      <c r="A16" s="59">
+        <f t="shared" ref="A16:A19" si="0">A15+1</f>
+        <v>3</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C16" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="184" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="67"/>
+      <c r="G16" s="152" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="59">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="C17" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="67"/>
+      <c r="G17" s="149"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="59">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="149" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="12" thickBot="1">
+      <c r="A19" s="72">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B19" s="256" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="68" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="257"/>
+      <c r="G19" s="258"/>
+    </row>
+    <row r="21" spans="1:7" ht="12" thickBot="1">
+      <c r="A21" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="207" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="208"/>
+      <c r="E22" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" s="35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="13">
+      <c r="A23" s="14">
+        <v>1</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="221" t="s">
+        <v>152</v>
+      </c>
+      <c r="D23" s="222"/>
+      <c r="E23" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="46" t="s">
+        <v>3</v>
+      </c>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="1:7" ht="13" customHeight="1">
+      <c r="A24" s="57">
+        <v>2</v>
+      </c>
+      <c r="B24" s="51"/>
+      <c r="C24" s="226"/>
+      <c r="D24" s="227"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="52"/>
+      <c r="G24" s="53"/>
+    </row>
+    <row r="25" spans="1:7" ht="13" customHeight="1" thickBot="1">
+      <c r="A25" s="56">
+        <v>3</v>
+      </c>
+      <c r="B25" s="54"/>
+      <c r="C25" s="224"/>
+      <c r="D25" s="225"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="55"/>
+    </row>
+    <row r="27" spans="1:7" ht="12" thickBot="1">
+      <c r="A27" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14" thickBot="1">
+      <c r="A28" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="209" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="210"/>
+      <c r="E28" s="209" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="223"/>
+      <c r="G28" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="14" thickBot="1">
+      <c r="A29" s="56">
+        <v>1</v>
+      </c>
+      <c r="B29" s="54"/>
+      <c r="C29" s="238" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="239"/>
+      <c r="E29" s="260" t="s">
+        <v>110</v>
+      </c>
+      <c r="F29" s="261"/>
+      <c r="G29" s="55" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="12" thickBot="1">
+      <c r="A31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14" thickBot="1">
+      <c r="A32" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="209" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="210"/>
+      <c r="E32" s="209" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="223"/>
+      <c r="G32" s="38" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="22">
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
+  <headerFooter>
+    <oddHeader>&amp;Lテーブル定義書&amp;R&amp;D</oddHeader>
+    <oddFooter>&amp;C&amp;P/&amp;N</oddFooter>
+  </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FF008000"/>
@@ -10253,103 +11209,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="210" t="s">
+      <c r="C2" s="200" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="215"/>
+      <c r="D2" s="201"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="210" t="s">
+      <c r="F2" s="200" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="211"/>
+      <c r="G2" s="204"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
+      <c r="C3" s="202"/>
+      <c r="D3" s="203"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="214" t="s">
+      <c r="F3" s="202" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="213"/>
+      <c r="G3" s="206"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="214" t="s">
+      <c r="C4" s="202" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="216"/>
+      <c r="D4" s="203"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="214"/>
-      <c r="G4" s="213"/>
+      <c r="F4" s="202"/>
+      <c r="G4" s="206"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="214" t="s">
+      <c r="C5" s="202" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="216"/>
+      <c r="D5" s="203"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="214"/>
-      <c r="G5" s="213"/>
+      <c r="F5" s="202"/>
+      <c r="G5" s="206"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="214" t="s">
+      <c r="C6" s="202" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="216"/>
+      <c r="D6" s="203"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="214"/>
-      <c r="G6" s="213"/>
+      <c r="F6" s="202"/>
+      <c r="G6" s="206"/>
     </row>
     <row r="7" spans="1:11" ht="13">
-      <c r="B7" s="198" t="s">
+      <c r="B7" s="211" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="200"/>
+      <c r="C7" s="212"/>
+      <c r="D7" s="212"/>
+      <c r="E7" s="212"/>
+      <c r="F7" s="212"/>
+      <c r="G7" s="213"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="201"/>
-      <c r="C8" s="202"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="203"/>
+      <c r="B8" s="214"/>
+      <c r="C8" s="215"/>
+      <c r="D8" s="215"/>
+      <c r="E8" s="215"/>
+      <c r="F8" s="215"/>
+      <c r="G8" s="216"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="204"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="203"/>
+      <c r="B9" s="217"/>
+      <c r="C9" s="215"/>
+      <c r="D9" s="215"/>
+      <c r="E9" s="215"/>
+      <c r="F9" s="215"/>
+      <c r="G9" s="216"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1">
-      <c r="B10" s="205"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="207"/>
+      <c r="B10" s="218"/>
+      <c r="C10" s="219"/>
+      <c r="D10" s="219"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="220"/>
     </row>
     <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -10571,10 +11527,10 @@
       <c r="B24" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="196" t="s">
+      <c r="C24" s="207" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="197"/>
+      <c r="D24" s="208"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -10592,10 +11548,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="208" t="s">
+      <c r="C25" s="221" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="209"/>
+      <c r="D25" s="222"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -10609,10 +11565,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="241" t="s">
+      <c r="C26" s="252" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="242"/>
+      <c r="D26" s="253"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -10631,14 +11587,14 @@
       <c r="B29" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="189" t="s">
+      <c r="C29" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="190"/>
-      <c r="E29" s="189" t="s">
+      <c r="D29" s="210"/>
+      <c r="E29" s="209" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="191"/>
+      <c r="F29" s="223"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -10655,14 +11611,14 @@
       <c r="B32" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="189" t="s">
+      <c r="C32" s="209" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="190"/>
-      <c r="E32" s="189" t="s">
+      <c r="D32" s="210"/>
+      <c r="E32" s="209" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="191"/>
+      <c r="F32" s="223"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -10672,20 +11628,29 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="239" t="s">
+      <c r="C33" s="250" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="240"/>
-      <c r="E33" s="241" t="s">
+      <c r="D33" s="251"/>
+      <c r="E33" s="252" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="242"/>
+      <c r="F33" s="253"/>
       <c r="G33" s="28" t="s">
         <v>50</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -10698,395 +11663,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
-  </mergeCells>
-  <phoneticPr fontId="2"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
-  <headerFooter>
-    <oddHeader>&amp;Lテーブル定義書&amp;R&amp;D</oddHeader>
-    <oddFooter>&amp;C&amp;P/&amp;N</oddFooter>
-  </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <tabColor rgb="FF008000"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:G28"/>
-  <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="3.6640625" style="13" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="18" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" style="18" customWidth="1"/>
-    <col min="5" max="6" width="10.1640625" style="18" customWidth="1"/>
-    <col min="7" max="7" width="28.6640625" style="18" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="13"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="12" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="13">
-      <c r="B2" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="210" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="215"/>
-      <c r="E2" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="210" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="211"/>
-    </row>
-    <row r="3" spans="1:7" ht="13">
-      <c r="B3" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="214"/>
-      <c r="D3" s="216"/>
-      <c r="E3" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="214" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="213"/>
-    </row>
-    <row r="4" spans="1:7" ht="13">
-      <c r="B4" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="214" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="216"/>
-      <c r="E4" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="214"/>
-      <c r="G4" s="213"/>
-    </row>
-    <row r="5" spans="1:7" ht="13">
-      <c r="B5" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="214" t="s">
-        <v>91</v>
-      </c>
-      <c r="D5" s="216"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="214"/>
-      <c r="G5" s="213"/>
-    </row>
-    <row r="6" spans="1:7" ht="13">
-      <c r="B6" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="214" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="216"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="214"/>
-      <c r="G6" s="213"/>
-    </row>
-    <row r="7" spans="1:7" ht="13">
-      <c r="B7" s="198" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="199"/>
-      <c r="D7" s="199"/>
-      <c r="E7" s="199"/>
-      <c r="F7" s="199"/>
-      <c r="G7" s="200"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="201" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="202"/>
-      <c r="D8" s="202"/>
-      <c r="E8" s="202"/>
-      <c r="F8" s="202"/>
-      <c r="G8" s="203"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="B9" s="204"/>
-      <c r="C9" s="202"/>
-      <c r="D9" s="202"/>
-      <c r="E9" s="202"/>
-      <c r="F9" s="202"/>
-      <c r="G9" s="203"/>
-    </row>
-    <row r="10" spans="1:7" ht="12" thickBot="1">
-      <c r="B10" s="205"/>
-      <c r="C10" s="206"/>
-      <c r="D10" s="206"/>
-      <c r="E10" s="206"/>
-      <c r="F10" s="206"/>
-      <c r="G10" s="207"/>
-    </row>
-    <row r="12" spans="1:7" ht="12" thickBot="1">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="14">
-        <v>1</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="74" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="15">
-        <f>A14+1</f>
-        <v>2</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="61" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="24"/>
-    </row>
-    <row r="16" spans="1:7" ht="12" thickBot="1">
-      <c r="A16" s="16">
-        <f t="shared" ref="A16" si="0">A15+1</f>
-        <v>3</v>
-      </c>
-      <c r="B16" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C16" s="62" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="28"/>
-    </row>
-    <row r="18" spans="1:7" ht="12" thickBot="1">
-      <c r="A18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="196" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" s="197"/>
-      <c r="E19" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="13">
-      <c r="A20" s="14">
-        <v>1</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="208" t="s">
-        <v>63</v>
-      </c>
-      <c r="D20" s="209"/>
-      <c r="E20" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="1:7" ht="14" thickBot="1">
-      <c r="A21" s="16">
-        <v>2</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="239" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="240"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="28"/>
-    </row>
-    <row r="23" spans="1:7" ht="12" thickBot="1">
-      <c r="A23" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="14" thickBot="1">
-      <c r="A24" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="189" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="190"/>
-      <c r="E24" s="189" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="191"/>
-      <c r="G24" s="38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="12" thickBot="1">
-      <c r="A26" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="14" thickBot="1">
-      <c r="A27" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="C27" s="189" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="190"/>
-      <c r="E27" s="189" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="191"/>
-      <c r="G27" s="38" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="14" thickBot="1">
-      <c r="A28" s="16">
-        <v>1</v>
-      </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="239"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="241"/>
-      <c r="F28" s="242"/>
-      <c r="G28" s="28"/>
-    </row>
-  </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>